<commit_message>
Placebo & Parallel Trends Tests
</commit_message>
<xml_diff>
--- a/data/multifamily_shares_calculations.xlsx
+++ b/data/multifamily_shares_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acec52acfc7c884e/Desktop/realpage-collusion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="8_{7A9D40F1-09DA-4C43-B533-2CF17A583C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87D25FF1-A00A-4A03-9A33-3010E55F8068}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{7A9D40F1-09DA-4C43-B533-2CF17A583C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C40963-8329-4A76-8677-59EDA435934F}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="2160" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{2AF12E00-6AAF-406B-B3EE-D4387BB46A4D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2AF12E00-6AAF-406B-B3EE-D4387BB46A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metro Area Share Gain" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3745,7 +3745,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -3795,10 +3795,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5543,7 +5543,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{5C54A94E-C292-4FAA-8F14-47FCBDA51C5E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5581,6 +5581,10 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5902,8 +5906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC209B8-60BA-41AA-BBC0-96C3F9E5EC9B}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -5961,7 +5965,7 @@
         <v>0.11899999999999999</v>
       </c>
       <c r="E2" s="1">
-        <f>SUM(C2:D2)</f>
+        <f t="shared" ref="E2:E21" si="0">SUM(C2:D2)</f>
         <v>0.33299999999999996</v>
       </c>
       <c r="F2" s="6">
@@ -5973,15 +5977,15 @@
         <v>472272.07140805805</v>
       </c>
       <c r="H2" s="1">
-        <f>C2*$F2/$G2</f>
+        <f t="shared" ref="H2:H21" si="1">C2*$F2/$G2</f>
         <v>0.40038773876041844</v>
       </c>
       <c r="I2" s="1">
-        <f>D2*$F2/$G2</f>
+        <f t="shared" ref="I2:I21" si="2">D2*$F2/$G2</f>
         <v>0.22264551828266257</v>
       </c>
       <c r="J2" s="4">
-        <f>SUM($H2:$I2)</f>
+        <f t="shared" ref="J2:J21" si="3">SUM($H2:$I2)</f>
         <v>0.62303325704308099</v>
       </c>
     </row>
@@ -5999,7 +6003,7 @@
         <v>0.104</v>
       </c>
       <c r="E3" s="1">
-        <f>SUM(C3:D3)</f>
+        <f t="shared" si="0"/>
         <v>0.32600000000000001</v>
       </c>
       <c r="F3" s="6">
@@ -6011,15 +6015,15 @@
         <v>738323.48850100464</v>
       </c>
       <c r="H3" s="1">
-        <f>C3*$F3/$G3</f>
+        <f t="shared" si="1"/>
         <v>0.33203624178597513</v>
       </c>
       <c r="I3" s="1">
-        <f>D3*$F3/$G3</f>
+        <f t="shared" si="2"/>
         <v>0.15554850966550185</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM($H3:$I3)</f>
+        <f t="shared" si="3"/>
         <v>0.48758475145147695</v>
       </c>
     </row>
@@ -6037,7 +6041,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="E4" s="1">
-        <f>SUM(C4:D4)</f>
+        <f t="shared" si="0"/>
         <v>0.217</v>
       </c>
       <c r="F4" s="6">
@@ -6049,15 +6053,15 @@
         <v>350280.61713821231</v>
       </c>
       <c r="H4" s="1">
-        <f>C4*$F4/$G4</f>
+        <f t="shared" si="1"/>
         <v>0.30940510432163754</v>
       </c>
       <c r="I4" s="1">
-        <f>D4*$F4/$G4</f>
+        <f t="shared" si="2"/>
         <v>0.14424967701481753</v>
       </c>
       <c r="J4" s="4">
-        <f>SUM($H4:$I4)</f>
+        <f t="shared" si="3"/>
         <v>0.45365478133645509</v>
       </c>
     </row>
@@ -6075,7 +6079,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="E5" s="1">
-        <f>SUM(C5:D5)</f>
+        <f t="shared" si="0"/>
         <v>0.32299999999999995</v>
       </c>
       <c r="F5" s="6">
@@ -6087,15 +6091,15 @@
         <v>344848.33900912991</v>
       </c>
       <c r="H5" s="1">
-        <f>C5*$F5/$G5</f>
+        <f t="shared" si="1"/>
         <v>0.31129606018877393</v>
       </c>
       <c r="I5" s="1">
-        <f>D5*$F5/$G5</f>
+        <f t="shared" si="2"/>
         <v>0.1165704395600515</v>
       </c>
       <c r="J5" s="4">
-        <f>SUM($H5:$I5)</f>
+        <f t="shared" si="3"/>
         <v>0.4278664997488254</v>
       </c>
     </row>
@@ -6113,7 +6117,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E6" s="1">
-        <f>SUM(C6:D6)</f>
+        <f t="shared" si="0"/>
         <v>0.223</v>
       </c>
       <c r="F6" s="6">
@@ -6125,15 +6129,15 @@
         <v>299574.74586803495</v>
       </c>
       <c r="H6" s="1">
-        <f>C6*$F6/$G6</f>
+        <f t="shared" si="1"/>
         <v>0.27391501189453354</v>
       </c>
       <c r="I6" s="1">
-        <f>D6*$F6/$G6</f>
+        <f t="shared" si="2"/>
         <v>0.12532059367723761</v>
       </c>
       <c r="J6" s="4">
-        <f>SUM($H6:$I6)</f>
+        <f t="shared" si="3"/>
         <v>0.39923560557177118</v>
       </c>
     </row>
@@ -6151,7 +6155,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E7" s="1">
-        <f>SUM(C7:D7)</f>
+        <f t="shared" si="0"/>
         <v>0.29900000000000004</v>
       </c>
       <c r="F7" s="6">
@@ -6163,15 +6167,15 @@
         <v>713417.10307337926</v>
       </c>
       <c r="H7" s="1">
-        <f>C7*$F7/$G7</f>
+        <f t="shared" si="1"/>
         <v>0.20511540952741419</v>
       </c>
       <c r="I7" s="1">
-        <f>D7*$F7/$G7</f>
+        <f t="shared" si="2"/>
         <v>0.16433945462136199</v>
       </c>
       <c r="J7" s="4">
-        <f>SUM($H7:$I7)</f>
+        <f t="shared" si="3"/>
         <v>0.36945486414877615</v>
       </c>
     </row>
@@ -6189,7 +6193,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="E8" s="1">
-        <f>SUM(C8:D8)</f>
+        <f t="shared" si="0"/>
         <v>0.217</v>
       </c>
       <c r="F8" s="6">
@@ -6201,15 +6205,15 @@
         <v>673724.11851393559</v>
       </c>
       <c r="H8" s="1">
-        <f>C8*$F8/$G8</f>
+        <f t="shared" si="1"/>
         <v>0.24472142714871709</v>
       </c>
       <c r="I8" s="1">
-        <f>D8*$F8/$G8</f>
+        <f t="shared" si="2"/>
         <v>8.9269451412739564E-2</v>
       </c>
       <c r="J8" s="4">
-        <f>SUM($H8:$I8)</f>
+        <f t="shared" si="3"/>
         <v>0.33399087856145665</v>
       </c>
     </row>
@@ -6227,7 +6231,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E9" s="1">
-        <f>SUM(C9:D9)</f>
+        <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
       <c r="F9" s="6">
@@ -6239,15 +6243,15 @@
         <v>175252.09442308225</v>
       </c>
       <c r="H9" s="1">
-        <f>C9*$F9/$G9</f>
+        <f t="shared" si="1"/>
         <v>0.2327506314367872</v>
       </c>
       <c r="I9" s="1">
-        <f>D9*$F9/$G9</f>
+        <f t="shared" si="2"/>
         <v>5.8187657859196801E-2</v>
       </c>
       <c r="J9" s="4">
-        <f>SUM($H9:$I9)</f>
+        <f t="shared" si="3"/>
         <v>0.29093828929598398</v>
       </c>
     </row>
@@ -6265,7 +6269,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="E10" s="1">
-        <f>SUM(C10:D10)</f>
+        <f t="shared" si="0"/>
         <v>0.158</v>
       </c>
       <c r="F10" s="6">
@@ -6277,15 +6281,15 @@
         <v>197961.65693723343</v>
       </c>
       <c r="H10" s="1">
-        <f>C10*$F10/$G10</f>
+        <f t="shared" si="1"/>
         <v>0.20160962274053157</v>
       </c>
       <c r="I10" s="1">
-        <f>D10*$F10/$G10</f>
+        <f t="shared" si="2"/>
         <v>6.6073741906560776E-2</v>
       </c>
       <c r="J10" s="4">
-        <f>SUM($H10:$I10)</f>
+        <f t="shared" si="3"/>
         <v>0.26768336464709236</v>
       </c>
     </row>
@@ -6303,7 +6307,7 @@
         <v>6.3E-2</v>
       </c>
       <c r="E11" s="1">
-        <f>SUM(C11:D11)</f>
+        <f t="shared" si="0"/>
         <v>0.17399999999999999</v>
       </c>
       <c r="F11" s="6">
@@ -6315,15 +6319,15 @@
         <v>462807.87233559729</v>
       </c>
       <c r="H11" s="1">
-        <f>C11*$F11/$G11</f>
+        <f t="shared" si="1"/>
         <v>0.1448054792664501</v>
       </c>
       <c r="I11" s="1">
-        <f>D11*$F11/$G11</f>
+        <f t="shared" si="2"/>
         <v>8.218689363771492E-2</v>
       </c>
       <c r="J11" s="4">
-        <f>SUM($H11:$I11)</f>
+        <f t="shared" si="3"/>
         <v>0.22699237290416502</v>
       </c>
     </row>
@@ -6341,7 +6345,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="E12" s="1">
-        <f>SUM(C12:D12)</f>
+        <f t="shared" si="0"/>
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="F12" s="6">
@@ -6353,15 +6357,15 @@
         <v>418443.34712875157</v>
       </c>
       <c r="H12" s="1">
-        <f>C12*$F12/$G12</f>
+        <f t="shared" si="1"/>
         <v>7.2580039278837244E-2</v>
       </c>
       <c r="I12" s="1">
-        <f>D12*$F12/$G12</f>
+        <f t="shared" si="2"/>
         <v>0.13636249803902753</v>
       </c>
       <c r="J12" s="4">
-        <f>SUM($H12:$I12)</f>
+        <f t="shared" si="3"/>
         <v>0.20894253731786477</v>
       </c>
     </row>
@@ -6379,7 +6383,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="E13" s="1">
-        <f>SUM(C13:D13)</f>
+        <f t="shared" si="0"/>
         <v>0.13100000000000001</v>
       </c>
       <c r="F13" s="6">
@@ -6391,15 +6395,15 @@
         <v>476595.84618527384</v>
       </c>
       <c r="H13" s="1">
-        <f>C13*$F13/$G13</f>
+        <f t="shared" si="1"/>
         <v>0.12105430719931595</v>
       </c>
       <c r="I13" s="1">
-        <f>D13*$F13/$G13</f>
+        <f t="shared" si="2"/>
         <v>7.7172120839563915E-2</v>
       </c>
       <c r="J13" s="4">
-        <f>SUM($H13:$I13)</f>
+        <f t="shared" si="3"/>
         <v>0.19822642803887985</v>
       </c>
     </row>
@@ -6417,7 +6421,7 @@
         <v>0.03</v>
       </c>
       <c r="E14" s="1">
-        <f>SUM(C14:D14)</f>
+        <f t="shared" si="0"/>
         <v>0.10199999999999999</v>
       </c>
       <c r="F14" s="6">
@@ -6429,15 +6433,15 @@
         <v>334317.25741350616</v>
       </c>
       <c r="H14" s="1">
-        <f>C14*$F14/$G14</f>
+        <f t="shared" si="1"/>
         <v>0.11807005215687226</v>
       </c>
       <c r="I14" s="1">
-        <f>D14*$F14/$G14</f>
+        <f t="shared" si="2"/>
         <v>4.919585506536344E-2</v>
       </c>
       <c r="J14" s="4">
-        <f>SUM($H14:$I14)</f>
+        <f t="shared" si="3"/>
         <v>0.16726590722223569</v>
       </c>
     </row>
@@ -6455,7 +6459,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E15" s="1">
-        <f>SUM(C15:D15)</f>
+        <f t="shared" si="0"/>
         <v>0.11599999999999999</v>
       </c>
       <c r="F15" s="6">
@@ -6467,15 +6471,15 @@
         <v>329772.9644263034</v>
       </c>
       <c r="H15" s="1">
-        <f>C15*$F15/$G15</f>
+        <f t="shared" si="1"/>
         <v>0.12122496947946973</v>
       </c>
       <c r="I15" s="1">
-        <f>D15*$F15/$G15</f>
+        <f t="shared" si="2"/>
         <v>3.3303563043810373E-2</v>
       </c>
       <c r="J15" s="4">
-        <f>SUM($H15:$I15)</f>
+        <f t="shared" si="3"/>
         <v>0.15452853252328011</v>
       </c>
     </row>
@@ -6493,7 +6497,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="E16" s="1">
-        <f>SUM(C16:D16)</f>
+        <f t="shared" si="0"/>
         <v>0.13899999999999998</v>
       </c>
       <c r="F16" s="6">
@@ -6505,15 +6509,15 @@
         <v>939398.95474776893</v>
       </c>
       <c r="H16" s="1">
-        <f>C16*$F16/$G16</f>
+        <f t="shared" si="1"/>
         <v>0.10199999999999999</v>
       </c>
       <c r="I16" s="1">
-        <f>D16*$F16/$G16</f>
+        <f t="shared" si="2"/>
         <v>3.7000000000000005E-2</v>
       </c>
       <c r="J16" s="4">
-        <f>SUM($H16:$I16)</f>
+        <f t="shared" si="3"/>
         <v>0.13900000000000001</v>
       </c>
     </row>
@@ -6531,7 +6535,7 @@
         <v>0.04</v>
       </c>
       <c r="E17" s="1">
-        <f>SUM(C17:D17)</f>
+        <f t="shared" si="0"/>
         <v>0.10100000000000001</v>
       </c>
       <c r="F17" s="6">
@@ -6543,15 +6547,15 @@
         <v>500463.28514518694</v>
       </c>
       <c r="H17" s="1">
-        <f>C17*$F17/$G17</f>
+        <f t="shared" si="1"/>
         <v>8.049624576017031E-2</v>
       </c>
       <c r="I17" s="1">
-        <f>D17*$F17/$G17</f>
+        <f t="shared" si="2"/>
         <v>5.2784423449292003E-2</v>
       </c>
       <c r="J17" s="4">
-        <f>SUM($H17:$I17)</f>
+        <f t="shared" si="3"/>
         <v>0.1332806692094623</v>
       </c>
     </row>
@@ -6569,7 +6573,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="E18" s="1">
-        <f>SUM(C18:D18)</f>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="F18" s="6">
@@ -6581,15 +6585,15 @@
         <v>908852.46745487314</v>
       </c>
       <c r="H18" s="1">
-        <f>C18*$F18/$G18</f>
+        <f t="shared" si="1"/>
         <v>8.3905287805068812E-2</v>
       </c>
       <c r="I18" s="1">
-        <f>D18*$F18/$G18</f>
+        <f t="shared" si="2"/>
         <v>3.5959409059315203E-2</v>
       </c>
       <c r="J18" s="4">
-        <f>SUM($H18:$I18)</f>
+        <f t="shared" si="3"/>
         <v>0.11986469686438402</v>
       </c>
     </row>
@@ -6607,7 +6611,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E19" s="1">
-        <f>SUM(C19:D19)</f>
+        <f t="shared" si="0"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F19" s="6">
@@ -6619,15 +6623,15 @@
         <v>268714.78064478911</v>
       </c>
       <c r="H19" s="1">
-        <f>C19*$F19/$G19</f>
+        <f t="shared" si="1"/>
         <v>5.0115975162763789E-2</v>
       </c>
       <c r="I19" s="1">
-        <f>D19*$F19/$G19</f>
+        <f t="shared" si="2"/>
         <v>4.5104377646487399E-2</v>
       </c>
       <c r="J19" s="4">
-        <f>SUM($H19:$I19)</f>
+        <f t="shared" si="3"/>
         <v>9.5220352809251188E-2</v>
       </c>
     </row>
@@ -6645,7 +6649,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E20" s="1">
-        <f>SUM(C20:D20)</f>
+        <f t="shared" si="0"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F20" s="6">
@@ -6657,15 +6661,15 @@
         <v>1439231.6302077468</v>
       </c>
       <c r="H20" s="1">
-        <f>C20*$F20/$G20</f>
+        <f t="shared" si="1"/>
         <v>4.7885870056802914E-2</v>
       </c>
       <c r="I20" s="1">
-        <f>D20*$F20/$G20</f>
+        <f t="shared" si="2"/>
         <v>2.9198701254148116E-2</v>
       </c>
       <c r="J20" s="4">
-        <f>SUM($H20:$I20)</f>
+        <f t="shared" si="3"/>
         <v>7.7084571310951033E-2</v>
       </c>
     </row>
@@ -6683,7 +6687,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="E21" s="1">
-        <f>SUM(C21:D21)</f>
+        <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F21" s="6">
@@ -6695,15 +6699,15 @@
         <v>2813891.1885221908</v>
       </c>
       <c r="H21" s="1">
-        <f>C21*$F21/$G21</f>
+        <f t="shared" si="1"/>
         <v>1.3999999999999999E-2</v>
       </c>
       <c r="I21" s="1">
-        <f>D21*$F21/$G21</f>
+        <f t="shared" si="2"/>
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="J21" s="4">
-        <f>SUM($H21:$I21)</f>
+        <f t="shared" si="3"/>
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
@@ -6805,7 +6809,7 @@
         <v>12583</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F5:F68" si="0">D8/B8</f>
+        <f t="shared" ref="F8:F68" si="0">D8/B8</f>
         <v>0.1475821301650227</v>
       </c>
       <c r="H8" t="s">

</xml_diff>

<commit_message>
Final presentation & paper upload
</commit_message>
<xml_diff>
--- a/data/multifamily_shares_calculations.xlsx
+++ b/data/multifamily_shares_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/acec52acfc7c884e/Desktop/realpage-collusion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{7A9D40F1-09DA-4C43-B533-2CF17A583C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C40963-8329-4A76-8677-59EDA435934F}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="8_{7A9D40F1-09DA-4C43-B533-2CF17A583C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B30E108E-4B74-4071-A6DE-F2A3DE9E06F4}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2AF12E00-6AAF-406B-B3EE-D4387BB46A4D}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="2" xr2:uid="{2AF12E00-6AAF-406B-B3EE-D4387BB46A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metro Area Share Gain" sheetId="5" r:id="rId1"/>
@@ -3920,76 +3920,204 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>rp_shares_all_units!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.1999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.0999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.6000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -4012,76 +4140,204 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>rp_shares_all_units!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.11899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -4104,76 +4360,204 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>rp_shares_all_units!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.33299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.217</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.217</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.11599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5999999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -4196,76 +4580,204 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>rp_shares_all_units!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>883607.22780734219</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1104279.9835323612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>732287.91140200105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>456808.20977099927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>536326.92861271021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>881523.14012504602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1036947.9735046648</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>566528.27274433128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>335386.34430425352</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>603757.7996562362</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>920322.25971433078</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>721174.74967537588</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>548234.11138548842</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>439304.58843662514</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>939398.95474776893</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>660416.64909818291</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1361741.5688240726</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>673345.16363308846</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1680947.7762382629</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2813891.1885221908</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -4288,76 +4800,204 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>rp_shares_all_units!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>472272.07140805805</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>738323.48850100464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>350280.61713821231</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>344848.33900912991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299574.74586803495</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>713417.10307337926</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>673724.11851393559</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175252.09442308225</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197961.65693723343</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>462807.87233559729</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>418443.34712875157</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>476595.84618527384</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>334317.25741350616</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>329772.9644263034</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>939398.95474776893</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>500463.28514518694</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>908852.46745487314</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>268714.78064478911</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1439231.6302077468</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2813891.1885221908</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -4383,72 +5023,136 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4544,72 +5248,136 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:multiLvlStrRef>
               <c:f>rp_shares_all_units!$A$2:$B$21</c:f>
-              <c:strCache>
+              <c:multiLvlStrCache>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>Atlanta, GA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dallas, TX</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Phoenix, AZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Denver, CO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Tampa, FL</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Washington, DC</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Houston, TX</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Riverside, CA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Las Vegas, NV</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Seattle, WA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Philadelphia, PA</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Boston, MA</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Minneapolis, MN</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>San Diego, CA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Miami, FL</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>San Francisco, CA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Chicago, IL</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Detroit, MI</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Los Angeles, CA</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>New York, NY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta-Sandy Springs-Roswell, GA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas-Fort Worth-Arlington, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix-Mesa-Chandler, AZ Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver-Aurora-Centennial, CO Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa-St. Petersburg-Clearwater, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington-Arlington-Alexandria, DC-VA-MD-WV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston-Pasadena-The Woodlands, TX Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside-San Bernardino-Ontario, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas-Henderson-North Las Vegas, NV Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle-Tacoma-Bellevue, WA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia-Camden-Wilmington, PA-NJ-DE-MD Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston-Cambridge-Newton, MA-NH Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis-St. Paul-Bloomington, MN-WI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego-Chula Vista-Carlsbad, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami-Fort Lauderdale-West Palm Beach, FL Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco-Oakland-Fremont, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago-Naperville-Elgin, IL-IN Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit-Warren-Dearborn, MI Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles-Long Beach-Anaheim, CA Metro Area</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York-Newark-Jersey City, NY-NJ Metro Area</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Atlanta, GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dallas, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Phoenix, AZ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Denver, CO</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Tampa, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Washington, DC</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Houston, TX</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Riverside, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Las Vegas, NV</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Seattle, WA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Philadelphia, PA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Boston, MA</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Minneapolis, MN</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>San Diego, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Miami, FL</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>San Francisco, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Chicago, IL</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Detroit, MI</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Los Angeles, CA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>New York, NY</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -5543,7 +6311,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{5C54A94E-C292-4FAA-8F14-47FCBDA51C5E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="47" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5554,7 +6322,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654815" cy="6274741"/>
+    <xdr:ext cx="8673830" cy="6290553"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5906,17 +6674,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC209B8-60BA-41AA-BBC0-96C3F9E5EC9B}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="5" width="8.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="12.77734375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="13.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -6723,7 +7490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F30F84-79BC-4976-A797-AAA058B39CC5}">
   <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>